<commit_message>
New Plotter Assembly and Pencil Holder
</commit_message>
<xml_diff>
--- a/Cost Estimate.xlsx
+++ b/Cost Estimate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa\Documents\PlotSomething\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA3CC36-AFF3-4632-AD3C-EA7758C6B3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADEA863-1661-4E08-BD5C-ED6F4F01F2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{87914853-9D23-4A52-83CB-A1AB6492AA98}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>#3/8-24 Zinc Plated Machine Screw Nut</t>
   </si>
   <si>
-    <t>https://www.homedepot.com/p/Everbilt-3-8-in-24-tpi-Zinc-Plated-Grade-5-Hex-Nut-851858/204836072</t>
-  </si>
-  <si>
     <t>3/8 in. Bearings for Screw and Shaft</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>Obtained Yet?</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/p/Everbilt-10-24-Stainless-Steel-Machine-Screw-Nut-4-Pack-800031/204274134</t>
   </si>
 </sst>
 </file>
@@ -679,7 +679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181D703F-20ED-4372-AC32-B179828F1B52}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -717,7 +719,7 @@
         <v>18</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>12</v>
@@ -737,20 +739,20 @@
         <v>2</v>
       </c>
       <c r="E2" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F2" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G2" s="16">
-        <f>0.33*6</f>
-        <v>1.98</v>
+        <f>2*1.28</f>
+        <v>2.56</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -761,7 +763,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -776,10 +778,10 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -806,10 +808,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>2</v>
@@ -827,15 +829,15 @@
         <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="14"/>
@@ -862,7 +864,7 @@
         <v>25.24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>13</v>
@@ -870,13 +872,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -888,18 +890,18 @@
         <v>12.99</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -917,15 +919,15 @@
         <v>3</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>3</v>
@@ -934,13 +936,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -952,42 +954,42 @@
         <v>11.95</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -1035,10 +1037,10 @@
     </row>
     <row r="21" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="14" t="s">
@@ -1048,34 +1050,34 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G24" s="21"/>
       <c r="I24" s="22"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="4">
         <v>27.13</v>
@@ -1083,13 +1085,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="4">
         <v>37.79</v>

</xml_diff>

<commit_message>
Cost Estimate and Solidworks Updates
</commit_message>
<xml_diff>
--- a/Cost Estimate.xlsx
+++ b/Cost Estimate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa\Documents\PlotSomething\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADEA863-1661-4E08-BD5C-ED6F4F01F2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C39CD9-BCF9-4E31-8F48-3CEE4938AF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{87914853-9D23-4A52-83CB-A1AB6492AA98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>Vendor</t>
   </si>
@@ -133,9 +133,6 @@
     <t>3/8 in. Base Shaft</t>
   </si>
   <si>
-    <t>Flange Bearing Mount</t>
-  </si>
-  <si>
     <t>https://www.homedepot.com/p/3-8-in-x-36-in-Plain-Steel-Round-Rod-802447/204273959</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>Alternatives if parts don't work out:</t>
   </si>
   <si>
-    <t>Base Shaft Mount</t>
-  </si>
-  <si>
     <t>Solenoid</t>
   </si>
   <si>
@@ -209,6 +203,9 @@
   </si>
   <si>
     <t>https://www.homedepot.com/p/Everbilt-10-24-Stainless-Steel-Machine-Screw-Nut-4-Pack-800031/204274134</t>
+  </si>
+  <si>
+    <t>36 in Metal Rod, 6 X 3/8-in nuts</t>
   </si>
 </sst>
 </file>
@@ -677,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181D703F-20ED-4372-AC32-B179828F1B52}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -719,7 +716,7 @@
         <v>18</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>12</v>
@@ -749,10 +746,10 @@
         <v>2.56</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -763,7 +760,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -778,10 +775,10 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -811,7 +808,7 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>2</v>
@@ -826,10 +823,10 @@
         <v>5.98</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -864,7 +861,7 @@
         <v>25.24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>13</v>
@@ -890,7 +887,7 @@
         <v>12.99</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>28</v>
@@ -901,7 +898,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -924,110 +921,120 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>11.95</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="10"/>
+        <v>53</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4">
-        <v>11.95</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
+      <c r="A16" t="s">
         <v>35</v>
       </c>
+      <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>37</v>
+    </row>
+    <row r="18" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="12">
+        <v>5</v>
+      </c>
+      <c r="F18" s="12">
+        <v>2</v>
+      </c>
+      <c r="G18" s="13">
+        <f>1.28*2</f>
+        <v>2.56</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="12">
-        <v>5</v>
-      </c>
-      <c r="F19" s="12">
         <v>2</v>
       </c>
-      <c r="G19" s="13">
-        <f>1.28*2</f>
-        <v>2.56</v>
-      </c>
+      <c r="G19" s="13"/>
       <c r="H19" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="15" t="s">
-        <v>21</v>
-      </c>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="14" t="s">
@@ -1035,66 +1042,67 @@
       </c>
       <c r="I20" s="15"/>
     </row>
-    <row r="21" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="20" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="20" t="s">
+      <c r="G23" s="21"/>
+      <c r="I23" s="22"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
         <v>49</v>
       </c>
-      <c r="G24" s="21"/>
-      <c r="I24" s="22"/>
+      <c r="D24" s="4">
+        <v>27.13</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D25" s="4">
-        <v>27.13</v>
+        <v>37.79</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D26" s="4">
-        <v>37.79</v>
+        <v>7.55</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -1105,9 +1113,6 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D30" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>